<commit_message>
Include controllers of getAllCars and postCar
</commit_message>
<xml_diff>
--- a/04_documentation/Mockup.xlsx
+++ b/04_documentation/Mockup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="18915" windowHeight="11835" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="18915" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="clienteEscritorio" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>Elementos</t>
   </si>
@@ -26,19 +26,7 @@
     <t>Carrusel</t>
   </si>
   <si>
-    <t>Objeto coche</t>
-  </si>
-  <si>
     <t>Navegador</t>
-  </si>
-  <si>
-    <t>Página detallada</t>
-  </si>
-  <si>
-    <t>Formulario contacto</t>
-  </si>
-  <si>
-    <t>Formulario Login</t>
   </si>
   <si>
     <t>Formulario confirmación</t>
@@ -188,6 +176,44 @@
   <si>
     <t>Comentarios</t>
   </si>
+  <si>
+    <t>Carruseles</t>
+  </si>
+  <si>
+    <t>Datos</t>
+  </si>
+  <si>
+    <t>Modelo y marca de todos los coches</t>
+  </si>
+  <si>
+    <t>Página 
+detallada</t>
+  </si>
+  <si>
+    <t>Foto, marca, modelo, 
+precio, kms,descripción, cilindrada</t>
+  </si>
+  <si>
+    <t>2 Carruseles con foto,marca,modelo, precio, kms, coches oferta</t>
+  </si>
+  <si>
+    <t>Foto, marca, modelo, precio, kms, coche oferta alquiler o venta</t>
+  </si>
+  <si>
+    <t>Formulario 
+contacto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre, apellidos, telefono,
+consulta </t>
+  </si>
+  <si>
+    <t>Formulario 
+Login</t>
+  </si>
+  <si>
+    <t>usuario, contraseña</t>
+  </si>
 </sst>
 </file>
 
@@ -241,7 +267,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -352,11 +378,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -377,6 +432,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -399,16 +456,56 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3688,7 +3785,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>522084</xdr:colOff>
+      <xdr:colOff>174702</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
@@ -24586,151 +24683,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C39:AL41"/>
+  <dimension ref="C38:AL42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="Q10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AH38" sqref="AH38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="21" max="21" width="16.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="38" spans="3:38" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="J38" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="22"/>
+      <c r="O38" s="22"/>
+      <c r="P38" s="22"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="22"/>
+      <c r="S38" s="22"/>
+      <c r="T38" s="22"/>
+      <c r="V38" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB38" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH38" s="35" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="39" spans="3:38" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="9" t="s">
-        <v>13</v>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="11" t="s">
+        <v>9</v>
       </c>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="9"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="9"/>
-      <c r="R39" s="9"/>
-      <c r="S39" s="9"/>
-      <c r="T39" s="9"/>
-      <c r="U39" s="8" t="s">
-        <v>4</v>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="20" t="s">
+        <v>54</v>
       </c>
-      <c r="V39" s="8"/>
-      <c r="W39" s="8"/>
-      <c r="X39" s="8"/>
-      <c r="Y39" s="8"/>
-      <c r="Z39" s="8" t="s">
-        <v>5</v>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="20"/>
+      <c r="O39" s="20"/>
+      <c r="P39" s="20"/>
+      <c r="Q39" s="20"/>
+      <c r="R39" s="20"/>
+      <c r="S39" s="20"/>
+      <c r="T39" s="21"/>
+      <c r="U39" s="25" t="s">
+        <v>55</v>
       </c>
-      <c r="AA39" s="8"/>
-      <c r="AB39" s="8"/>
-      <c r="AC39" s="8"/>
-      <c r="AD39" s="8"/>
-      <c r="AE39" s="8"/>
-      <c r="AF39" s="8" t="s">
-        <v>6</v>
+      <c r="V39" s="29" t="s">
+        <v>56</v>
       </c>
-      <c r="AG39" s="8"/>
-      <c r="AH39" s="8"/>
-      <c r="AI39" s="8"/>
-      <c r="AJ39" s="8"/>
-      <c r="AK39" s="8"/>
-      <c r="AL39" s="8"/>
+      <c r="W39" s="10"/>
+      <c r="X39" s="10"/>
+      <c r="Y39" s="10"/>
+      <c r="Z39" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA39" s="29"/>
+      <c r="AB39" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC39" s="28"/>
+      <c r="AD39" s="28"/>
+      <c r="AE39" s="32"/>
+      <c r="AF39" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG39" s="29"/>
+      <c r="AH39" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI39" s="2"/>
+      <c r="AJ39" s="2"/>
+      <c r="AK39" s="2"/>
+      <c r="AL39" s="3"/>
     </row>
     <row r="40" spans="3:38" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="9" t="s">
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="20"/>
+      <c r="P40" s="20"/>
+      <c r="Q40" s="20"/>
+      <c r="R40" s="20"/>
+      <c r="S40" s="20"/>
+      <c r="T40" s="21"/>
+      <c r="U40" s="26"/>
+      <c r="V40" s="10"/>
+      <c r="W40" s="10"/>
+      <c r="X40" s="10"/>
+      <c r="Y40" s="10"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="26"/>
+      <c r="AC40" s="30"/>
+      <c r="AD40" s="30"/>
+      <c r="AE40" s="33"/>
+      <c r="AF40" s="29"/>
+      <c r="AG40" s="29"/>
+      <c r="AH40" s="23"/>
+      <c r="AI40" s="23"/>
+      <c r="AJ40" s="23"/>
+      <c r="AK40" s="23"/>
+      <c r="AL40" s="24"/>
+    </row>
+    <row r="41" spans="3:38" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
-      <c r="N40" s="9"/>
-      <c r="O40" s="9"/>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="9"/>
-      <c r="R40" s="9"/>
-      <c r="S40" s="9"/>
-      <c r="T40" s="9"/>
-      <c r="U40" s="8"/>
-      <c r="V40" s="8"/>
-      <c r="W40" s="8"/>
-      <c r="X40" s="8"/>
-      <c r="Y40" s="8"/>
-      <c r="Z40" s="8"/>
-      <c r="AA40" s="8"/>
-      <c r="AB40" s="8"/>
-      <c r="AC40" s="8"/>
-      <c r="AD40" s="8"/>
-      <c r="AE40" s="8"/>
-      <c r="AF40" s="8"/>
-      <c r="AG40" s="8"/>
-      <c r="AH40" s="8"/>
-      <c r="AI40" s="8"/>
-      <c r="AJ40" s="8"/>
-      <c r="AK40" s="8"/>
-      <c r="AL40" s="8"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="K41" s="20"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="20"/>
+      <c r="P41" s="20"/>
+      <c r="Q41" s="20"/>
+      <c r="R41" s="20"/>
+      <c r="S41" s="20"/>
+      <c r="T41" s="21"/>
+      <c r="U41" s="26"/>
+      <c r="V41" s="10"/>
+      <c r="W41" s="10"/>
+      <c r="X41" s="10"/>
+      <c r="Y41" s="10"/>
+      <c r="Z41" s="29"/>
+      <c r="AA41" s="29"/>
+      <c r="AB41" s="26"/>
+      <c r="AC41" s="30"/>
+      <c r="AD41" s="30"/>
+      <c r="AE41" s="33"/>
+      <c r="AF41" s="29"/>
+      <c r="AG41" s="29"/>
+      <c r="AH41" s="23"/>
+      <c r="AI41" s="23"/>
+      <c r="AJ41" s="23"/>
+      <c r="AK41" s="23"/>
+      <c r="AL41" s="24"/>
     </row>
-    <row r="41" spans="3:38" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
-      <c r="N41" s="9"/>
-      <c r="O41" s="9"/>
-      <c r="P41" s="9"/>
-      <c r="Q41" s="9"/>
-      <c r="R41" s="9"/>
-      <c r="S41" s="9"/>
-      <c r="T41" s="9"/>
-      <c r="U41" s="8"/>
-      <c r="V41" s="8"/>
-      <c r="W41" s="8"/>
-      <c r="X41" s="8"/>
-      <c r="Y41" s="8"/>
-      <c r="Z41" s="8"/>
-      <c r="AA41" s="8"/>
-      <c r="AB41" s="8"/>
-      <c r="AC41" s="8"/>
-      <c r="AD41" s="8"/>
-      <c r="AE41" s="8"/>
-      <c r="AF41" s="8"/>
-      <c r="AG41" s="8"/>
-      <c r="AH41" s="8"/>
-      <c r="AI41" s="8"/>
-      <c r="AJ41" s="8"/>
-      <c r="AK41" s="8"/>
-      <c r="AL41" s="8"/>
+    <row r="42" spans="3:38" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="20"/>
+      <c r="O42" s="20"/>
+      <c r="P42" s="20"/>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="20"/>
+      <c r="S42" s="20"/>
+      <c r="T42" s="21"/>
+      <c r="U42" s="27"/>
+      <c r="V42" s="10"/>
+      <c r="W42" s="10"/>
+      <c r="X42" s="10"/>
+      <c r="Y42" s="10"/>
+      <c r="Z42" s="29"/>
+      <c r="AA42" s="29"/>
+      <c r="AB42" s="27"/>
+      <c r="AC42" s="31"/>
+      <c r="AD42" s="31"/>
+      <c r="AE42" s="34"/>
+      <c r="AF42" s="29"/>
+      <c r="AG42" s="29"/>
+      <c r="AH42" s="4"/>
+      <c r="AI42" s="4"/>
+      <c r="AJ42" s="4"/>
+      <c r="AK42" s="4"/>
+      <c r="AL42" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="AF39:AL41"/>
-    <mergeCell ref="G39:T39"/>
-    <mergeCell ref="G40:T40"/>
-    <mergeCell ref="G41:T41"/>
-    <mergeCell ref="C39:F41"/>
-    <mergeCell ref="U39:Y41"/>
-    <mergeCell ref="Z39:AE41"/>
+  <mergeCells count="11">
+    <mergeCell ref="J38:T38"/>
+    <mergeCell ref="U39:U42"/>
+    <mergeCell ref="V39:Y42"/>
+    <mergeCell ref="Z39:AA42"/>
+    <mergeCell ref="AB39:AE42"/>
+    <mergeCell ref="C39:F42"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="AF39:AG42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -24749,154 +24927,159 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="35" spans="3:17" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="12" t="s">
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
     </row>
     <row r="36" spans="3:17" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="12" t="s">
-        <v>8</v>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="14" t="s">
+        <v>4</v>
       </c>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
     </row>
     <row r="72" spans="3:31" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C72" s="11" t="s">
+      <c r="C72" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D72" s="11"/>
-      <c r="E72" s="11"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
       <c r="F72" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
       <c r="J72" s="3"/>
-      <c r="K72" s="9" t="s">
-        <v>10</v>
+      <c r="K72" s="11" t="s">
+        <v>6</v>
       </c>
-      <c r="L72" s="9"/>
-      <c r="M72" s="9"/>
-      <c r="N72" s="9"/>
-      <c r="O72" s="9"/>
-      <c r="P72" s="9"/>
-      <c r="Q72" s="9"/>
-      <c r="R72" s="8" t="s">
-        <v>12</v>
+      <c r="L72" s="11"/>
+      <c r="M72" s="11"/>
+      <c r="N72" s="11"/>
+      <c r="O72" s="11"/>
+      <c r="P72" s="11"/>
+      <c r="Q72" s="11"/>
+      <c r="R72" s="10" t="s">
+        <v>8</v>
       </c>
-      <c r="S72" s="8"/>
-      <c r="T72" s="8"/>
-      <c r="U72" s="8"/>
-      <c r="V72" s="8"/>
-      <c r="W72" s="8"/>
-      <c r="X72" s="8"/>
-      <c r="Y72" s="9" t="s">
-        <v>10</v>
+      <c r="S72" s="10"/>
+      <c r="T72" s="10"/>
+      <c r="U72" s="10"/>
+      <c r="V72" s="10"/>
+      <c r="W72" s="10"/>
+      <c r="X72" s="10"/>
+      <c r="Y72" s="11" t="s">
+        <v>6</v>
       </c>
-      <c r="Z72" s="9"/>
-      <c r="AA72" s="9"/>
-      <c r="AB72" s="9"/>
-      <c r="AC72" s="9"/>
-      <c r="AD72" s="9"/>
-      <c r="AE72" s="9"/>
+      <c r="Z72" s="11"/>
+      <c r="AA72" s="11"/>
+      <c r="AB72" s="11"/>
+      <c r="AC72" s="11"/>
+      <c r="AD72" s="11"/>
+      <c r="AE72" s="11"/>
     </row>
     <row r="73" spans="3:31" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
       <c r="F73" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="J73" s="5"/>
-      <c r="K73" s="9" t="s">
+      <c r="K73" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="L73" s="11"/>
+      <c r="M73" s="11"/>
+      <c r="N73" s="11"/>
+      <c r="O73" s="11"/>
+      <c r="P73" s="11"/>
+      <c r="Q73" s="11"/>
+      <c r="R73" s="10"/>
+      <c r="S73" s="10"/>
+      <c r="T73" s="10"/>
+      <c r="U73" s="10"/>
+      <c r="V73" s="10"/>
+      <c r="W73" s="10"/>
+      <c r="X73" s="10"/>
+      <c r="Y73" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z73" s="11"/>
+      <c r="AA73" s="11"/>
+      <c r="AB73" s="11"/>
+      <c r="AC73" s="11"/>
+      <c r="AD73" s="11"/>
+      <c r="AE73" s="11"/>
+    </row>
+    <row r="74" spans="3:31" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="K74" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="L73" s="9"/>
-      <c r="M73" s="9"/>
-      <c r="N73" s="9"/>
-      <c r="O73" s="9"/>
-      <c r="P73" s="9"/>
-      <c r="Q73" s="9"/>
-      <c r="R73" s="8"/>
-      <c r="S73" s="8"/>
-      <c r="T73" s="8"/>
-      <c r="U73" s="8"/>
-      <c r="V73" s="8"/>
-      <c r="W73" s="8"/>
-      <c r="X73" s="8"/>
-      <c r="Y73" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z73" s="9"/>
-      <c r="AA73" s="9"/>
-      <c r="AB73" s="9"/>
-      <c r="AC73" s="9"/>
-      <c r="AD73" s="9"/>
-      <c r="AE73" s="9"/>
-    </row>
-    <row r="74" spans="3:31" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="K74" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L74" s="9"/>
-      <c r="M74" s="9"/>
-      <c r="N74" s="9"/>
-      <c r="O74" s="9"/>
-      <c r="P74" s="9"/>
-      <c r="Q74" s="9"/>
+      <c r="L74" s="11"/>
+      <c r="M74" s="11"/>
+      <c r="N74" s="11"/>
+      <c r="O74" s="11"/>
+      <c r="P74" s="11"/>
+      <c r="Q74" s="11"/>
     </row>
     <row r="75" spans="3:31" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="K75" s="9" t="s">
-        <v>16</v>
+      <c r="K75" s="11" t="s">
+        <v>12</v>
       </c>
-      <c r="L75" s="9"/>
-      <c r="M75" s="9"/>
-      <c r="N75" s="9"/>
-      <c r="O75" s="9"/>
-      <c r="P75" s="9"/>
-      <c r="Q75" s="9"/>
+      <c r="L75" s="11"/>
+      <c r="M75" s="11"/>
+      <c r="N75" s="11"/>
+      <c r="O75" s="11"/>
+      <c r="P75" s="11"/>
+      <c r="Q75" s="11"/>
     </row>
     <row r="77" spans="3:31" x14ac:dyDescent="0.25">
       <c r="K77" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="L35:Q36"/>
+    <mergeCell ref="C35:E36"/>
+    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="F36:K36"/>
+    <mergeCell ref="K72:Q72"/>
     <mergeCell ref="Y72:AE72"/>
     <mergeCell ref="Y73:AE73"/>
     <mergeCell ref="K74:Q74"/>
@@ -24904,11 +25087,6 @@
     <mergeCell ref="C72:E73"/>
     <mergeCell ref="R72:X73"/>
     <mergeCell ref="K73:Q73"/>
-    <mergeCell ref="L35:Q36"/>
-    <mergeCell ref="C35:E36"/>
-    <mergeCell ref="F35:K35"/>
-    <mergeCell ref="F36:K36"/>
-    <mergeCell ref="K72:Q72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -24935,8 +25113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24947,83 +25125,83 @@
   <sheetData>
     <row r="2" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="18" t="s">
-        <v>18</v>
+      <c r="B4" s="9" t="s">
+        <v>14</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>55</v>
+      <c r="C4" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
-        <v>19</v>
+      <c r="B5" s="18" t="s">
+        <v>15</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>22</v>
+      <c r="C5" s="18" t="s">
+        <v>18</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="8">
         <v>200</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="8">
         <v>404</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
-        <v>20</v>
+      <c r="B7" s="19" t="s">
+        <v>16</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>23</v>
+      <c r="C7" s="18" t="s">
+        <v>19</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="8">
         <v>201</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16">
+      <c r="B8" s="19"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="8">
         <v>400</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
-        <v>24</v>
+      <c r="B9" s="19" t="s">
+        <v>20</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>25</v>
+      <c r="C9" s="18" t="s">
+        <v>21</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="8">
         <v>201</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="17"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16">
+      <c r="B10" s="19"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="8">
         <v>400</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16">
+      <c r="B11" s="19"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="8">
         <v>401</v>
       </c>
     </row>
@@ -25031,257 +25209,263 @@
       <c r="B12" s="6"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="18" t="s">
-        <v>27</v>
+      <c r="B14" s="9" t="s">
+        <v>23</v>
       </c>
-      <c r="C14" s="18" t="s">
-        <v>55</v>
+      <c r="C14" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
-        <v>28</v>
+      <c r="B15" s="17" t="s">
+        <v>24</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>30</v>
+      <c r="C15" s="17" t="s">
+        <v>26</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="8">
         <v>201</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="16">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="8">
         <v>400</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="19" t="s">
-        <v>29</v>
+      <c r="B17" s="17" t="s">
+        <v>25</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>31</v>
+      <c r="C17" s="17" t="s">
+        <v>27</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="8">
         <v>201</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="16">
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="8">
         <v>400</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="19" t="s">
-        <v>32</v>
+      <c r="B19" s="17" t="s">
+        <v>28</v>
       </c>
-      <c r="C19" s="19" t="s">
-        <v>42</v>
+      <c r="C19" s="17" t="s">
+        <v>38</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="8">
         <v>201</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="16">
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="8">
         <v>400</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="19" t="s">
-        <v>26</v>
+      <c r="B21" s="17" t="s">
+        <v>22</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>43</v>
+      <c r="C21" s="17" t="s">
+        <v>39</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="8">
         <v>200</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="16">
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="8">
         <v>404</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="19" t="s">
-        <v>33</v>
+      <c r="B23" s="17" t="s">
+        <v>29</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>44</v>
+      <c r="C23" s="17" t="s">
+        <v>40</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="8">
         <v>201</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="16">
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="8">
         <v>400</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="19" t="s">
-        <v>34</v>
+      <c r="B25" s="17" t="s">
+        <v>30</v>
       </c>
-      <c r="C25" s="19" t="s">
-        <v>45</v>
+      <c r="C25" s="17" t="s">
+        <v>41</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="8">
         <v>201</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="16">
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="8">
         <v>400</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="19" t="s">
-        <v>35</v>
+      <c r="B27" s="17" t="s">
+        <v>31</v>
       </c>
-      <c r="C27" s="19" t="s">
-        <v>46</v>
+      <c r="C27" s="17" t="s">
+        <v>42</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="8">
         <v>200</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="16">
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="8">
         <v>404</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="19" t="s">
-        <v>36</v>
+      <c r="B29" s="17" t="s">
+        <v>32</v>
       </c>
-      <c r="C29" s="19" t="s">
-        <v>47</v>
+      <c r="C29" s="17" t="s">
+        <v>43</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="8">
         <v>201</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="16">
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="8">
         <v>400</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="19" t="s">
-        <v>37</v>
+      <c r="B31" s="17" t="s">
+        <v>33</v>
       </c>
-      <c r="C31" s="19" t="s">
-        <v>48</v>
+      <c r="C31" s="17" t="s">
+        <v>44</v>
       </c>
-      <c r="D31" s="16">
+      <c r="D31" s="8">
         <v>201</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="16">
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="8">
         <v>400</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="19" t="s">
-        <v>38</v>
+      <c r="B33" s="17" t="s">
+        <v>34</v>
       </c>
-      <c r="C33" s="19" t="s">
-        <v>49</v>
+      <c r="C33" s="17" t="s">
+        <v>45</v>
       </c>
-      <c r="D33" s="16">
+      <c r="D33" s="8">
         <v>200</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="16">
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="8">
         <v>404</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="19" t="s">
-        <v>39</v>
+      <c r="B35" s="17" t="s">
+        <v>35</v>
       </c>
-      <c r="C35" s="19" t="s">
-        <v>50</v>
+      <c r="C35" s="17" t="s">
+        <v>46</v>
       </c>
-      <c r="D35" s="16">
+      <c r="D35" s="8">
         <v>200</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="16">
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="8">
         <v>404</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="19" t="s">
-        <v>40</v>
+      <c r="B37" s="17" t="s">
+        <v>36</v>
       </c>
-      <c r="C37" s="19" t="s">
-        <v>51</v>
+      <c r="C37" s="17" t="s">
+        <v>47</v>
       </c>
-      <c r="D37" s="16">
+      <c r="D37" s="8">
         <v>200</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="16">
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="8">
         <v>404</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="19" t="s">
-        <v>41</v>
+      <c r="B39" s="17" t="s">
+        <v>37</v>
       </c>
-      <c r="C39" s="19" t="s">
-        <v>52</v>
+      <c r="C39" s="17" t="s">
+        <v>48</v>
       </c>
-      <c r="D39" s="16">
+      <c r="D39" s="8">
         <v>201</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="16">
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="8">
         <v>400</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="C33:C34"/>
     <mergeCell ref="C35:C36"/>
@@ -25298,17 +25482,11 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Improve format of Mockup
</commit_message>
<xml_diff>
--- a/04_documentation/Mockup.xlsx
+++ b/04_documentation/Mockup.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
   <si>
     <t>Elementos</t>
   </si>
@@ -158,9 +158,6 @@
 Login</t>
   </si>
   <si>
-    <t>usuario, contraseña</t>
-  </si>
-  <si>
     <t>Modelo y marca de todos los coches disponibles</t>
   </si>
   <si>
@@ -179,10 +176,6 @@
   <si>
     <t>Formulario 
 alta vehículo</t>
-  </si>
-  <si>
-    <t>matricula, modelo, marca, km, precio
-        , foto, cilindrada, combustible, alquiler, oferta</t>
   </si>
   <si>
     <t>Formulario 
@@ -295,12 +288,21 @@
   <si>
     <t>Registrar cliente</t>
   </si>
+  <si>
+    <t>Usuario, contraseña</t>
+  </si>
+  <si>
+    <t>matricula, modelo, marca, km, precio, foto, cilindrada, combustible, alquiler, oferta</t>
+  </si>
+  <si>
+    <t>DNI,nombre, apellidos, telefono, cpostal, ciudad</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,22 +358,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -386,13 +372,6 @@
     </font>
     <font>
       <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -583,20 +562,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -605,47 +572,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -663,8 +606,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -672,170 +663,117 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -28146,8 +28084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C38:AL42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB39" sqref="AB39:AE42"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28156,220 +28094,221 @@
   </cols>
   <sheetData>
     <row r="38" spans="3:38" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="J38" s="14" t="s">
+      <c r="J38" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
-      <c r="T38" s="14"/>
-      <c r="V38" s="13" t="s">
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
+      <c r="V38" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AB38" s="13" t="s">
+      <c r="AB38" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AH38" s="13" t="s">
+      <c r="AH38" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="39" spans="3:38" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="27" t="s">
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="9" t="s">
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="5"/>
+      <c r="S39" s="5"/>
+      <c r="T39" s="6"/>
+      <c r="U39" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="V39" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="W39" s="40"/>
+      <c r="X39" s="40"/>
+      <c r="Y39" s="41"/>
+      <c r="Z39" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA39" s="13"/>
+      <c r="AB39" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC39" s="52"/>
+      <c r="AD39" s="52"/>
+      <c r="AE39" s="53"/>
+      <c r="AF39" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG39" s="13"/>
+      <c r="AH39" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI39" s="40"/>
+      <c r="AJ39" s="40"/>
+      <c r="AK39" s="40"/>
+      <c r="AL39" s="41"/>
+    </row>
+    <row r="40" spans="3:38" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="9"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="9"/>
-      <c r="R39" s="9"/>
-      <c r="S39" s="9"/>
-      <c r="T39" s="10"/>
-      <c r="U39" s="15" t="s">
-        <v>39</v>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5"/>
+      <c r="S40" s="5"/>
+      <c r="T40" s="6"/>
+      <c r="U40" s="21"/>
+      <c r="V40" s="42"/>
+      <c r="W40" s="43"/>
+      <c r="X40" s="43"/>
+      <c r="Y40" s="44"/>
+      <c r="Z40" s="13"/>
+      <c r="AA40" s="13"/>
+      <c r="AB40" s="54"/>
+      <c r="AC40" s="55"/>
+      <c r="AD40" s="55"/>
+      <c r="AE40" s="56"/>
+      <c r="AF40" s="13"/>
+      <c r="AG40" s="13"/>
+      <c r="AH40" s="42"/>
+      <c r="AI40" s="43"/>
+      <c r="AJ40" s="43"/>
+      <c r="AK40" s="43"/>
+      <c r="AL40" s="44"/>
+    </row>
+    <row r="41" spans="3:38" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="16" t="s">
+        <v>1</v>
       </c>
-      <c r="V39" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="W39" s="19"/>
-      <c r="X39" s="19"/>
-      <c r="Y39" s="19"/>
-      <c r="Z39" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA39" s="18"/>
-      <c r="AB39" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC39" s="20"/>
-      <c r="AD39" s="20"/>
-      <c r="AE39" s="21"/>
-      <c r="AF39" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG39" s="18"/>
-      <c r="AH39" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI39" s="1"/>
-      <c r="AJ39" s="1"/>
-      <c r="AK39" s="1"/>
-      <c r="AL39" s="2"/>
-    </row>
-    <row r="40" spans="3:38" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="9" t="s">
+      <c r="H41" s="17"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
-      <c r="N40" s="9"/>
-      <c r="O40" s="9"/>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="9"/>
-      <c r="R40" s="9"/>
-      <c r="S40" s="9"/>
-      <c r="T40" s="10"/>
-      <c r="U40" s="16"/>
-      <c r="V40" s="19"/>
-      <c r="W40" s="19"/>
-      <c r="X40" s="19"/>
-      <c r="Y40" s="19"/>
-      <c r="Z40" s="18"/>
-      <c r="AA40" s="18"/>
-      <c r="AB40" s="16"/>
-      <c r="AC40" s="22"/>
-      <c r="AD40" s="22"/>
-      <c r="AE40" s="23"/>
-      <c r="AF40" s="18"/>
-      <c r="AG40" s="18"/>
-      <c r="AH40" s="11"/>
-      <c r="AI40" s="11"/>
-      <c r="AJ40" s="11"/>
-      <c r="AK40" s="11"/>
-      <c r="AL40" s="12"/>
-    </row>
-    <row r="41" spans="3:38" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="H41" s="29"/>
-      <c r="I41" s="30"/>
-      <c r="J41" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
-      <c r="N41" s="9"/>
-      <c r="O41" s="9"/>
-      <c r="P41" s="9"/>
-      <c r="Q41" s="9"/>
-      <c r="R41" s="9"/>
-      <c r="S41" s="9"/>
-      <c r="T41" s="10"/>
-      <c r="U41" s="16"/>
-      <c r="V41" s="19"/>
-      <c r="W41" s="19"/>
-      <c r="X41" s="19"/>
-      <c r="Y41" s="19"/>
-      <c r="Z41" s="18"/>
-      <c r="AA41" s="18"/>
-      <c r="AB41" s="16"/>
-      <c r="AC41" s="22"/>
-      <c r="AD41" s="22"/>
-      <c r="AE41" s="23"/>
-      <c r="AF41" s="18"/>
-      <c r="AG41" s="18"/>
-      <c r="AH41" s="11"/>
-      <c r="AI41" s="11"/>
-      <c r="AJ41" s="11"/>
-      <c r="AK41" s="11"/>
-      <c r="AL41" s="12"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5"/>
+      <c r="S41" s="5"/>
+      <c r="T41" s="6"/>
+      <c r="U41" s="21"/>
+      <c r="V41" s="42"/>
+      <c r="W41" s="43"/>
+      <c r="X41" s="43"/>
+      <c r="Y41" s="44"/>
+      <c r="Z41" s="13"/>
+      <c r="AA41" s="13"/>
+      <c r="AB41" s="54"/>
+      <c r="AC41" s="55"/>
+      <c r="AD41" s="55"/>
+      <c r="AE41" s="56"/>
+      <c r="AF41" s="13"/>
+      <c r="AG41" s="13"/>
+      <c r="AH41" s="42"/>
+      <c r="AI41" s="43"/>
+      <c r="AJ41" s="43"/>
+      <c r="AK41" s="43"/>
+      <c r="AL41" s="44"/>
     </row>
     <row r="42" spans="3:38" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="27"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
-      <c r="N42" s="9"/>
-      <c r="O42" s="9"/>
-      <c r="P42" s="9"/>
-      <c r="Q42" s="9"/>
-      <c r="R42" s="9"/>
-      <c r="S42" s="9"/>
-      <c r="T42" s="10"/>
-      <c r="U42" s="17"/>
-      <c r="V42" s="19"/>
-      <c r="W42" s="19"/>
-      <c r="X42" s="19"/>
-      <c r="Y42" s="19"/>
-      <c r="Z42" s="18"/>
-      <c r="AA42" s="18"/>
-      <c r="AB42" s="17"/>
-      <c r="AC42" s="24"/>
-      <c r="AD42" s="24"/>
-      <c r="AE42" s="25"/>
-      <c r="AF42" s="18"/>
-      <c r="AG42" s="18"/>
-      <c r="AH42" s="3"/>
-      <c r="AI42" s="3"/>
-      <c r="AJ42" s="3"/>
-      <c r="AK42" s="3"/>
-      <c r="AL42" s="4"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+      <c r="S42" s="5"/>
+      <c r="T42" s="6"/>
+      <c r="U42" s="22"/>
+      <c r="V42" s="45"/>
+      <c r="W42" s="46"/>
+      <c r="X42" s="46"/>
+      <c r="Y42" s="47"/>
+      <c r="Z42" s="13"/>
+      <c r="AA42" s="13"/>
+      <c r="AB42" s="57"/>
+      <c r="AC42" s="58"/>
+      <c r="AD42" s="58"/>
+      <c r="AE42" s="59"/>
+      <c r="AF42" s="13"/>
+      <c r="AG42" s="13"/>
+      <c r="AH42" s="45"/>
+      <c r="AI42" s="46"/>
+      <c r="AJ42" s="46"/>
+      <c r="AK42" s="46"/>
+      <c r="AL42" s="47"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="AH39:AL42"/>
+    <mergeCell ref="J38:T38"/>
+    <mergeCell ref="U39:U42"/>
+    <mergeCell ref="V39:Y42"/>
+    <mergeCell ref="Z39:AA42"/>
+    <mergeCell ref="AB39:AE42"/>
     <mergeCell ref="AF39:AG42"/>
     <mergeCell ref="C39:F42"/>
     <mergeCell ref="G39:I39"/>
     <mergeCell ref="G40:I40"/>
     <mergeCell ref="G41:I41"/>
     <mergeCell ref="G42:I42"/>
-    <mergeCell ref="J38:T38"/>
-    <mergeCell ref="U39:U42"/>
-    <mergeCell ref="V39:Y42"/>
-    <mergeCell ref="Z39:AA42"/>
-    <mergeCell ref="AB39:AE42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -28381,12 +28320,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C36:AS89"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView showGridLines="0" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
     <col min="40" max="40" width="14.85546875" customWidth="1"/>
   </cols>
@@ -28397,378 +28337,378 @@
       </c>
     </row>
     <row r="37" spans="3:17" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C37" s="31" t="s">
+      <c r="C37" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="35" t="s">
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G37" s="35"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="19" t="s">
+      <c r="G37" s="28"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="19"/>
+      <c r="M37" s="23"/>
+      <c r="N37" s="23"/>
+      <c r="O37" s="23"/>
+      <c r="P37" s="23"/>
+      <c r="Q37" s="23"/>
     </row>
     <row r="38" spans="3:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="36" t="s">
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" s="24"/>
+      <c r="H38" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="G38" s="36"/>
-      <c r="H38" s="37" t="s">
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="23"/>
+      <c r="N38" s="23"/>
+      <c r="O38" s="23"/>
+      <c r="P38" s="23"/>
+      <c r="Q38" s="23"/>
+    </row>
+    <row r="74" spans="3:45" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C74" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="26"/>
+      <c r="E74" s="27"/>
+      <c r="F74" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="I38" s="38"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="19"/>
-    </row>
-    <row r="74" spans="3:45" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C74" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="D74" s="31"/>
-      <c r="E74" s="41"/>
-      <c r="F74" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="G74" s="40"/>
-      <c r="H74" s="51" t="s">
-        <v>51</v>
+      <c r="G74" s="25"/>
+      <c r="H74" s="39" t="s">
+        <v>83</v>
       </c>
       <c r="I74" s="52"/>
       <c r="J74" s="53"/>
       <c r="K74" s="61" t="s">
+        <v>52</v>
+      </c>
+      <c r="L74" s="62"/>
+      <c r="M74" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="N74" s="75"/>
+      <c r="O74" s="75"/>
+      <c r="P74" s="75"/>
+      <c r="Q74" s="75"/>
+      <c r="R74" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="L74" s="62"/>
-      <c r="M74" s="68" t="s">
-        <v>51</v>
+      <c r="S74" s="25"/>
+      <c r="T74" s="74" t="s">
+        <v>59</v>
       </c>
-      <c r="N74" s="69"/>
-      <c r="O74" s="69"/>
-      <c r="P74" s="69"/>
-      <c r="Q74" s="69"/>
-      <c r="R74" s="70" t="s">
-        <v>56</v>
+      <c r="U74" s="75"/>
+      <c r="V74" s="75"/>
+      <c r="W74" s="75"/>
+      <c r="X74" s="75"/>
+      <c r="Y74" s="67" t="s">
+        <v>58</v>
       </c>
-      <c r="S74" s="70"/>
-      <c r="T74" s="68" t="s">
-        <v>61</v>
+      <c r="Z74" s="68"/>
+      <c r="AA74" s="39" t="s">
+        <v>83</v>
       </c>
-      <c r="U74" s="69"/>
-      <c r="V74" s="69"/>
-      <c r="W74" s="69"/>
-      <c r="X74" s="69"/>
-      <c r="Y74" s="72" t="s">
+      <c r="AB74" s="52"/>
+      <c r="AC74" s="52"/>
+      <c r="AD74" s="52"/>
+      <c r="AE74" s="53"/>
+      <c r="AF74" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="Z74" s="71"/>
-      <c r="AA74" s="77" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB74" s="78"/>
-      <c r="AC74" s="78"/>
-      <c r="AD74" s="78"/>
-      <c r="AE74" s="79"/>
-      <c r="AF74" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG74" s="71"/>
-      <c r="AH74" s="77" t="s">
+      <c r="AG74" s="68"/>
+      <c r="AH74" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="AI74" s="78"/>
-      <c r="AJ74" s="78"/>
-      <c r="AK74" s="78"/>
-      <c r="AL74" s="79"/>
-      <c r="AM74" s="72" t="s">
-        <v>70</v>
-      </c>
-      <c r="AN74" s="71"/>
-      <c r="AO74" s="77" t="s">
+      <c r="AI74" s="52"/>
+      <c r="AJ74" s="52"/>
+      <c r="AK74" s="52"/>
+      <c r="AL74" s="53"/>
+      <c r="AM74" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="AP74" s="78"/>
-      <c r="AQ74" s="78"/>
-      <c r="AR74" s="78"/>
-      <c r="AS74" s="79"/>
+      <c r="AN74" s="69"/>
+      <c r="AO74" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP74" s="52"/>
+      <c r="AQ74" s="52"/>
+      <c r="AR74" s="52"/>
+      <c r="AS74" s="53"/>
     </row>
     <row r="75" spans="3:45" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C75" s="31"/>
-      <c r="D75" s="31"/>
-      <c r="E75" s="41"/>
-      <c r="F75" s="40"/>
-      <c r="G75" s="40"/>
+      <c r="C75" s="26"/>
+      <c r="D75" s="26"/>
+      <c r="E75" s="27"/>
+      <c r="F75" s="25"/>
+      <c r="G75" s="25"/>
       <c r="H75" s="54"/>
       <c r="I75" s="55"/>
       <c r="J75" s="56"/>
       <c r="K75" s="63"/>
       <c r="L75" s="64"/>
-      <c r="M75" s="69"/>
-      <c r="N75" s="69"/>
-      <c r="O75" s="69"/>
-      <c r="P75" s="69"/>
-      <c r="Q75" s="69"/>
-      <c r="R75" s="70"/>
-      <c r="S75" s="70"/>
-      <c r="T75" s="69"/>
-      <c r="U75" s="69"/>
-      <c r="V75" s="69"/>
-      <c r="W75" s="69"/>
-      <c r="X75" s="69"/>
-      <c r="Y75" s="71"/>
-      <c r="Z75" s="71"/>
-      <c r="AA75" s="80"/>
-      <c r="AB75" s="81"/>
-      <c r="AC75" s="81"/>
-      <c r="AD75" s="81"/>
-      <c r="AE75" s="82"/>
-      <c r="AF75" s="71"/>
-      <c r="AG75" s="71"/>
-      <c r="AH75" s="80"/>
-      <c r="AI75" s="81"/>
-      <c r="AJ75" s="81"/>
-      <c r="AK75" s="81"/>
-      <c r="AL75" s="82"/>
-      <c r="AM75" s="71"/>
+      <c r="M75" s="75"/>
+      <c r="N75" s="75"/>
+      <c r="O75" s="75"/>
+      <c r="P75" s="75"/>
+      <c r="Q75" s="75"/>
+      <c r="R75" s="25"/>
+      <c r="S75" s="25"/>
+      <c r="T75" s="75"/>
+      <c r="U75" s="75"/>
+      <c r="V75" s="75"/>
+      <c r="W75" s="75"/>
+      <c r="X75" s="75"/>
+      <c r="Y75" s="68"/>
+      <c r="Z75" s="68"/>
+      <c r="AA75" s="54"/>
+      <c r="AB75" s="55"/>
+      <c r="AC75" s="55"/>
+      <c r="AD75" s="55"/>
+      <c r="AE75" s="56"/>
+      <c r="AF75" s="68"/>
+      <c r="AG75" s="68"/>
+      <c r="AH75" s="54"/>
+      <c r="AI75" s="55"/>
+      <c r="AJ75" s="55"/>
+      <c r="AK75" s="55"/>
+      <c r="AL75" s="56"/>
+      <c r="AM75" s="70"/>
       <c r="AN75" s="71"/>
-      <c r="AO75" s="80"/>
-      <c r="AP75" s="81"/>
-      <c r="AQ75" s="81"/>
-      <c r="AR75" s="81"/>
-      <c r="AS75" s="82"/>
+      <c r="AO75" s="54"/>
+      <c r="AP75" s="55"/>
+      <c r="AQ75" s="55"/>
+      <c r="AR75" s="55"/>
+      <c r="AS75" s="56"/>
     </row>
     <row r="76" spans="3:45" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F76" s="40"/>
-      <c r="G76" s="40"/>
+      <c r="F76" s="25"/>
+      <c r="G76" s="25"/>
       <c r="H76" s="57"/>
       <c r="I76" s="58"/>
       <c r="J76" s="59"/>
       <c r="K76" s="65"/>
       <c r="L76" s="66"/>
-      <c r="M76" s="69"/>
-      <c r="N76" s="69"/>
-      <c r="O76" s="69"/>
-      <c r="P76" s="69"/>
-      <c r="Q76" s="69"/>
-      <c r="R76" s="70"/>
-      <c r="S76" s="70"/>
-      <c r="T76" s="69"/>
-      <c r="U76" s="69"/>
-      <c r="V76" s="69"/>
-      <c r="W76" s="69"/>
-      <c r="X76" s="69"/>
-      <c r="Y76" s="71"/>
-      <c r="Z76" s="71"/>
-      <c r="AA76" s="83"/>
-      <c r="AB76" s="84"/>
-      <c r="AC76" s="84"/>
-      <c r="AD76" s="84"/>
-      <c r="AE76" s="85"/>
-      <c r="AF76" s="71"/>
-      <c r="AG76" s="71"/>
-      <c r="AH76" s="83"/>
-      <c r="AI76" s="84"/>
-      <c r="AJ76" s="84"/>
-      <c r="AK76" s="84"/>
-      <c r="AL76" s="85"/>
-      <c r="AM76" s="71"/>
-      <c r="AN76" s="71"/>
-      <c r="AO76" s="83"/>
-      <c r="AP76" s="84"/>
-      <c r="AQ76" s="84"/>
-      <c r="AR76" s="84"/>
-      <c r="AS76" s="85"/>
+      <c r="M76" s="75"/>
+      <c r="N76" s="75"/>
+      <c r="O76" s="75"/>
+      <c r="P76" s="75"/>
+      <c r="Q76" s="75"/>
+      <c r="R76" s="25"/>
+      <c r="S76" s="25"/>
+      <c r="T76" s="75"/>
+      <c r="U76" s="75"/>
+      <c r="V76" s="75"/>
+      <c r="W76" s="75"/>
+      <c r="X76" s="75"/>
+      <c r="Y76" s="68"/>
+      <c r="Z76" s="68"/>
+      <c r="AA76" s="57"/>
+      <c r="AB76" s="58"/>
+      <c r="AC76" s="58"/>
+      <c r="AD76" s="58"/>
+      <c r="AE76" s="59"/>
+      <c r="AF76" s="68"/>
+      <c r="AG76" s="68"/>
+      <c r="AH76" s="57"/>
+      <c r="AI76" s="58"/>
+      <c r="AJ76" s="58"/>
+      <c r="AK76" s="58"/>
+      <c r="AL76" s="59"/>
+      <c r="AM76" s="72"/>
+      <c r="AN76" s="73"/>
+      <c r="AO76" s="57"/>
+      <c r="AP76" s="58"/>
+      <c r="AQ76" s="58"/>
+      <c r="AR76" s="58"/>
+      <c r="AS76" s="59"/>
     </row>
     <row r="77" spans="3:45" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F77" s="40" t="s">
-        <v>52</v>
+      <c r="F77" s="48" t="s">
+        <v>50</v>
       </c>
-      <c r="G77" s="40"/>
-      <c r="H77" s="60" t="s">
+      <c r="G77" s="49"/>
+      <c r="H77" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I77" s="52"/>
+      <c r="J77" s="53"/>
+      <c r="K77" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="I77" s="60"/>
-      <c r="J77" s="67"/>
-      <c r="K77" s="36" t="s">
+      <c r="L77" s="67"/>
+      <c r="M77" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="N77" s="75"/>
+      <c r="O77" s="75"/>
+      <c r="P77" s="75"/>
+      <c r="Q77" s="75"/>
+      <c r="R77" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="L77" s="36"/>
-      <c r="M77" s="68" t="s">
-        <v>53</v>
+      <c r="S77" s="25"/>
+      <c r="T77" s="74" t="s">
+        <v>56</v>
       </c>
-      <c r="N77" s="69"/>
-      <c r="O77" s="69"/>
-      <c r="P77" s="69"/>
-      <c r="Q77" s="69"/>
-      <c r="R77" s="70" t="s">
+      <c r="U77" s="75"/>
+      <c r="V77" s="75"/>
+      <c r="W77" s="75"/>
+      <c r="X77" s="75"/>
+      <c r="Y77" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="S77" s="70"/>
-      <c r="T77" s="68" t="s">
-        <v>58</v>
+      <c r="Z77" s="67"/>
+      <c r="AA77" s="39" t="s">
+        <v>84</v>
       </c>
-      <c r="U77" s="69"/>
-      <c r="V77" s="69"/>
-      <c r="W77" s="69"/>
-      <c r="X77" s="69"/>
-      <c r="Y77" s="36" t="s">
-        <v>59</v>
+      <c r="AB77" s="52"/>
+      <c r="AC77" s="52"/>
+      <c r="AD77" s="52"/>
+      <c r="AE77" s="53"/>
+      <c r="AM77" s="48" t="s">
+        <v>67</v>
       </c>
-      <c r="Z77" s="36"/>
-      <c r="AA77" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB77" s="44"/>
-      <c r="AC77" s="44"/>
-      <c r="AD77" s="44"/>
-      <c r="AE77" s="73"/>
-      <c r="AM77" s="72" t="s">
+      <c r="AN77" s="69"/>
+      <c r="AO77" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="AN77" s="71"/>
-      <c r="AO77" s="77" t="s">
-        <v>71</v>
-      </c>
-      <c r="AP77" s="78"/>
-      <c r="AQ77" s="78"/>
-      <c r="AR77" s="78"/>
-      <c r="AS77" s="79"/>
+      <c r="AP77" s="52"/>
+      <c r="AQ77" s="52"/>
+      <c r="AR77" s="52"/>
+      <c r="AS77" s="53"/>
     </row>
     <row r="78" spans="3:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F78" s="45"/>
-      <c r="G78" s="46"/>
-      <c r="H78" s="49"/>
-      <c r="I78" s="50"/>
-      <c r="J78" s="50"/>
-      <c r="K78" s="36"/>
-      <c r="L78" s="36"/>
-      <c r="M78" s="69"/>
-      <c r="N78" s="69"/>
-      <c r="O78" s="69"/>
-      <c r="P78" s="69"/>
-      <c r="Q78" s="69"/>
-      <c r="R78" s="70"/>
-      <c r="S78" s="70"/>
-      <c r="T78" s="69"/>
-      <c r="U78" s="69"/>
-      <c r="V78" s="69"/>
-      <c r="W78" s="69"/>
-      <c r="X78" s="69"/>
-      <c r="Y78" s="36"/>
-      <c r="Z78" s="36"/>
-      <c r="AA78" s="74"/>
-      <c r="AB78" s="75"/>
-      <c r="AC78" s="75"/>
-      <c r="AD78" s="75"/>
-      <c r="AE78" s="76"/>
-      <c r="AM78" s="71"/>
+      <c r="F78" s="50"/>
+      <c r="G78" s="51"/>
+      <c r="H78" s="57"/>
+      <c r="I78" s="58"/>
+      <c r="J78" s="59"/>
+      <c r="K78" s="67"/>
+      <c r="L78" s="67"/>
+      <c r="M78" s="75"/>
+      <c r="N78" s="75"/>
+      <c r="O78" s="75"/>
+      <c r="P78" s="75"/>
+      <c r="Q78" s="75"/>
+      <c r="R78" s="25"/>
+      <c r="S78" s="25"/>
+      <c r="T78" s="75"/>
+      <c r="U78" s="75"/>
+      <c r="V78" s="75"/>
+      <c r="W78" s="75"/>
+      <c r="X78" s="75"/>
+      <c r="Y78" s="67"/>
+      <c r="Z78" s="67"/>
+      <c r="AA78" s="57"/>
+      <c r="AB78" s="58"/>
+      <c r="AC78" s="58"/>
+      <c r="AD78" s="58"/>
+      <c r="AE78" s="59"/>
+      <c r="AM78" s="70"/>
       <c r="AN78" s="71"/>
-      <c r="AO78" s="80"/>
-      <c r="AP78" s="81"/>
-      <c r="AQ78" s="81"/>
-      <c r="AR78" s="81"/>
-      <c r="AS78" s="82"/>
+      <c r="AO78" s="54"/>
+      <c r="AP78" s="55"/>
+      <c r="AQ78" s="55"/>
+      <c r="AR78" s="55"/>
+      <c r="AS78" s="56"/>
     </row>
     <row r="79" spans="3:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F79" s="47"/>
-      <c r="G79" s="48"/>
-      <c r="H79" s="49"/>
-      <c r="I79" s="50"/>
-      <c r="J79" s="50"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="10"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="12"/>
       <c r="K79" t="s">
         <v>5</v>
       </c>
-      <c r="R79" s="70"/>
-      <c r="S79" s="70"/>
-      <c r="AM79" s="71"/>
-      <c r="AN79" s="71"/>
-      <c r="AO79" s="83"/>
-      <c r="AP79" s="84"/>
-      <c r="AQ79" s="84"/>
-      <c r="AR79" s="84"/>
-      <c r="AS79" s="85"/>
+      <c r="R79" s="25"/>
+      <c r="S79" s="25"/>
+      <c r="AM79" s="72"/>
+      <c r="AN79" s="73"/>
+      <c r="AO79" s="57"/>
+      <c r="AP79" s="58"/>
+      <c r="AQ79" s="58"/>
+      <c r="AR79" s="58"/>
+      <c r="AS79" s="59"/>
     </row>
     <row r="80" spans="3:45" x14ac:dyDescent="0.25">
-      <c r="AQ80" s="42"/>
+      <c r="AQ80" s="8"/>
     </row>
     <row r="81" spans="8:43" x14ac:dyDescent="0.25">
-      <c r="AQ81" s="42"/>
+      <c r="AQ81" s="8"/>
     </row>
     <row r="82" spans="8:43" x14ac:dyDescent="0.25">
-      <c r="AQ82" s="42"/>
+      <c r="AQ82" s="8"/>
     </row>
     <row r="83" spans="8:43" x14ac:dyDescent="0.25">
-      <c r="AQ83" s="42"/>
+      <c r="AQ83" s="8"/>
     </row>
     <row r="84" spans="8:43" x14ac:dyDescent="0.25">
-      <c r="H84" s="42"/>
-      <c r="AQ84" s="42"/>
+      <c r="H84" s="8"/>
+      <c r="AQ84" s="8"/>
     </row>
     <row r="85" spans="8:43" x14ac:dyDescent="0.25">
-      <c r="H85" s="42"/>
-      <c r="AQ85" s="42"/>
+      <c r="H85" s="8"/>
+      <c r="AQ85" s="8"/>
     </row>
     <row r="86" spans="8:43" x14ac:dyDescent="0.25">
-      <c r="H86" s="42"/>
+      <c r="H86" s="8"/>
     </row>
     <row r="87" spans="8:43" x14ac:dyDescent="0.25">
-      <c r="H87" s="42"/>
+      <c r="H87" s="8"/>
     </row>
     <row r="88" spans="8:43" x14ac:dyDescent="0.25">
-      <c r="H88" s="42"/>
+      <c r="H88" s="8"/>
     </row>
     <row r="89" spans="8:43" x14ac:dyDescent="0.25">
-      <c r="H89" s="42"/>
+      <c r="H89" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="L37:Q38"/>
+    <mergeCell ref="C37:E38"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="C74:E75"/>
+    <mergeCell ref="H74:J76"/>
+    <mergeCell ref="F74:G76"/>
+    <mergeCell ref="H77:J78"/>
+    <mergeCell ref="F77:G78"/>
+    <mergeCell ref="K77:L78"/>
+    <mergeCell ref="M77:Q78"/>
+    <mergeCell ref="R74:S76"/>
+    <mergeCell ref="R77:S79"/>
+    <mergeCell ref="T74:X76"/>
+    <mergeCell ref="T77:X78"/>
+    <mergeCell ref="K74:L76"/>
+    <mergeCell ref="Y77:Z78"/>
+    <mergeCell ref="Y74:Z76"/>
+    <mergeCell ref="AA74:AE76"/>
+    <mergeCell ref="AA77:AE78"/>
+    <mergeCell ref="M74:Q76"/>
     <mergeCell ref="AF74:AG76"/>
     <mergeCell ref="AH74:AL76"/>
     <mergeCell ref="AM74:AN76"/>
     <mergeCell ref="AO74:AS76"/>
     <mergeCell ref="AM77:AN79"/>
     <mergeCell ref="AO77:AS79"/>
-    <mergeCell ref="Y77:Z78"/>
-    <mergeCell ref="Y74:Z76"/>
-    <mergeCell ref="AA74:AE76"/>
-    <mergeCell ref="AA77:AE78"/>
-    <mergeCell ref="M74:Q76"/>
-    <mergeCell ref="K77:L78"/>
-    <mergeCell ref="M77:Q78"/>
-    <mergeCell ref="R74:S76"/>
-    <mergeCell ref="R77:S79"/>
-    <mergeCell ref="T74:X76"/>
-    <mergeCell ref="T77:X78"/>
-    <mergeCell ref="C74:E75"/>
-    <mergeCell ref="H74:J76"/>
-    <mergeCell ref="F74:G76"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="H77:J77"/>
-    <mergeCell ref="K74:L76"/>
-    <mergeCell ref="L37:Q38"/>
-    <mergeCell ref="C37:E38"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H38:K38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -28795,8 +28735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28806,7 +28746,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
@@ -28819,82 +28759,82 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="3">
         <v>200</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="7">
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="3">
         <v>404</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="3">
         <v>201</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="33"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="7">
+      <c r="B8" s="37"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="3">
         <v>400</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="3">
         <v>201</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="33"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="7">
+      <c r="B10" s="37"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="3">
         <v>400</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="33"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="7">
+      <c r="B11" s="37"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="3">
         <v>401</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
+      <c r="B12" s="1"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D14" t="s">
@@ -28902,346 +28842,339 @@
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="34" t="s">
-        <v>72</v>
+      <c r="B15" s="33" t="s">
+        <v>70</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="3">
         <v>201</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="7">
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="3">
         <v>400</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="34" t="s">
-        <v>73</v>
+      <c r="B17" s="33" t="s">
+        <v>71</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="3">
         <v>201</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="7">
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="3">
         <v>400</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="87" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="7">
+      <c r="D19" s="3">
         <v>200</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="34"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="7">
+      <c r="B20" s="33"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="3">
         <v>404</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="87" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="7">
+      <c r="D21" s="3">
         <v>200</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="34"/>
-      <c r="C22" s="88"/>
-      <c r="D22" s="7">
+      <c r="B22" s="33"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="3">
         <v>404</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="87" t="s">
+      <c r="B23" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="87" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" s="7">
+      <c r="D23" s="3">
         <v>201</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="88"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="7">
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="3">
         <v>400</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="87" t="s">
+      <c r="B25" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="87" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="7">
+      <c r="D25" s="3">
         <v>201</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="88"/>
-      <c r="C26" s="88"/>
-      <c r="D26" s="7">
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="3">
         <v>400</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="86" t="s">
-        <v>67</v>
+      <c r="B27" s="32" t="s">
+        <v>65</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="3">
         <v>201</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="86"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="7">
+      <c r="B28" s="32"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="3">
         <v>400</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="86" t="s">
-        <v>65</v>
+      <c r="B29" s="32" t="s">
+        <v>63</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="3">
         <v>200</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="86"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="7">
+      <c r="B30" s="32"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="3">
         <v>404</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="86" t="s">
-        <v>64</v>
+      <c r="B31" s="32" t="s">
+        <v>62</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="3">
         <v>201</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="86"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="7">
+      <c r="B32" s="32"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="3">
         <v>400</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="86" t="s">
-        <v>63</v>
+      <c r="B33" s="32" t="s">
+        <v>61</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="3">
         <v>201</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="86"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="7">
+      <c r="B34" s="32"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="3">
         <v>400</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="86" t="s">
+      <c r="B35" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="3">
         <v>200</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="86"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="7">
+      <c r="B36" s="32"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="3">
         <v>404</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="86" t="s">
-        <v>82</v>
+      <c r="B37" s="32" t="s">
+        <v>80</v>
       </c>
-      <c r="C37" s="34" t="s">
-        <v>83</v>
+      <c r="C37" s="33" t="s">
+        <v>81</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="3">
         <v>201</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="86"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="7">
+      <c r="B38" s="32"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="3">
         <v>400</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="86" t="s">
+      <c r="B39" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C39" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="3">
         <v>201</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="86"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="7">
+      <c r="B40" s="32"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="3">
         <v>400</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="34" t="s">
+      <c r="B41" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="34" t="s">
+      <c r="C41" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D41" s="3">
         <v>201</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="7">
+      <c r="B42" s="33"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="3">
         <v>400</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="86" t="s">
-        <v>66</v>
+      <c r="B43" s="32" t="s">
+        <v>64</v>
       </c>
-      <c r="C43" s="34" t="s">
+      <c r="C43" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D43" s="3">
         <v>200</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="86"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="7">
+      <c r="B44" s="32"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="3">
         <v>404</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="86" t="s">
+      <c r="B45" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="34" t="s">
+      <c r="C45" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="3">
         <v>200</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="86"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="7">
+      <c r="B46" s="32"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="3">
         <v>404</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="34" t="s">
+      <c r="B47" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C47" s="34" t="s">
+      <c r="C47" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="3">
         <v>200</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="34"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="7">
+      <c r="B48" s="33"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="3">
         <v>404</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="34" t="s">
+      <c r="B49" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C49" s="34" t="s">
+      <c r="C49" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D49" s="3">
         <v>201</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="34"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="7">
+      <c r="B50" s="33"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="3">
         <v>400</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C5:C6"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="C43:C44"/>
     <mergeCell ref="C45:C46"/>
@@ -29258,17 +29191,24 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="C29:C30"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="C33:C34"/>
     <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>